<commit_message>
Fixed typos and minor bugs with later versions of Perl modules. Added missing module MetagDB::Utils.
</commit_message>
<xml_diff>
--- a/bin/tests/data/spreadsheets/test_SGA_Kraken2.xlsx
+++ b/bin/tests/data/spreadsheets/test_SGA_Kraken2.xlsx
@@ -115,7 +115,7 @@
     <t xml:space="preserve">meconium</t>
   </si>
   <si>
-    <t xml:space="preserve">Kraken2</t>
+    <t xml:space="preserve">Kraken 2</t>
   </si>
   <si>
     <t xml:space="preserve">RDP</t>
@@ -398,7 +398,7 @@
   <dimension ref="A1:AB754"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z29" activeCellId="0" sqref="Z29"/>
+      <selection pane="topLeft" activeCell="Z3" activeCellId="0" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,7 +684,7 @@
       </c>
       <c r="Z3" s="8" t="str">
         <f aca="false">$Z2</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>32</v>
@@ -778,7 +778,7 @@
       </c>
       <c r="Z4" s="8" t="str">
         <f aca="false">$Z3</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA4" s="8" t="s">
         <v>32</v>
@@ -872,7 +872,7 @@
       </c>
       <c r="Z5" s="8" t="str">
         <f aca="false">$Z4</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA5" s="8" t="s">
         <v>32</v>
@@ -966,7 +966,7 @@
       </c>
       <c r="Z6" s="8" t="str">
         <f aca="false">$Z5</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>32</v>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="Z7" s="8" t="str">
         <f aca="false">$Z6</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA7" s="8" t="s">
         <v>32</v>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="Z8" s="8" t="str">
         <f aca="false">$Z7</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA8" s="8" t="s">
         <v>32</v>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="Z9" s="8" t="str">
         <f aca="false">$Z8</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA9" s="8" t="s">
         <v>32</v>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="Z10" s="8" t="str">
         <f aca="false">$Z9</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA10" s="8" t="s">
         <v>32</v>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="Z11" s="8" t="str">
         <f aca="false">$Z10</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA11" s="8" t="s">
         <v>32</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="Z12" s="8" t="str">
         <f aca="false">$Z11</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA12" s="8" t="s">
         <v>32</v>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="Z13" s="8" t="str">
         <f aca="false">$Z12</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA13" s="8" t="s">
         <v>32</v>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="Z14" s="8" t="str">
         <f aca="false">$Z13</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA14" s="8" t="s">
         <v>32</v>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="Z15" s="8" t="str">
         <f aca="false">$Z14</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA15" s="8" t="s">
         <v>32</v>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="Z16" s="8" t="str">
         <f aca="false">$Z15</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA16" s="8" t="s">
         <v>32</v>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="Z17" s="8" t="str">
         <f aca="false">$Z16</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA17" s="8" t="s">
         <v>32</v>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="Z18" s="8" t="str">
         <f aca="false">$Z17</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA18" s="8" t="s">
         <v>32</v>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="Z19" s="8" t="str">
         <f aca="false">$Z18</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA19" s="8" t="s">
         <v>32</v>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="Z20" s="8" t="str">
         <f aca="false">$Z19</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA20" s="8" t="s">
         <v>32</v>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="Z21" s="8" t="str">
         <f aca="false">$Z20</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA21" s="8" t="s">
         <v>32</v>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="Z22" s="8" t="str">
         <f aca="false">$Z21</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA22" s="8" t="s">
         <v>32</v>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="Z23" s="8" t="str">
         <f aca="false">$Z22</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA23" s="8" t="s">
         <v>32</v>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="Z24" s="8" t="str">
         <f aca="false">$Z23</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA24" s="8" t="s">
         <v>32</v>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="Z25" s="8" t="str">
         <f aca="false">$Z24</f>
-        <v>Kraken2</v>
+        <v>Kraken 2</v>
       </c>
       <c r="AA25" s="8" t="s">
         <v>32</v>

</xml_diff>